<commit_message>
Actualización del plan general Agrege los criterios de entrada y salida a casi todas las tareas existentes.
</commit_message>
<xml_diff>
--- a/tspi/ciclo-1/schedule/20095495.xlsx
+++ b/tspi/ciclo-1/schedule/20095495.xlsx
@@ -18,7 +18,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="27" uniqueCount="27">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="25" uniqueCount="25">
   <si>
     <t>Plan</t>
   </si>
@@ -29,9 +29,6 @@
     <t>Nombre</t>
   </si>
   <si>
-    <t>Pid</t>
-  </si>
-  <si>
     <t>Criterio de entrada</t>
   </si>
   <si>
@@ -96,18 +93,14 @@
   </si>
   <si>
     <t>Elaborar el reporte de cierre del ciclo #1 de TSPi.</t>
-  </si>
-  <si>
-    <t>Realizar el lanzamiento del ciclo #2 de TSPi.</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <numFmts count="2">
+  <numFmts count="1">
     <numFmt formatCode="GENERAL" numFmtId="164"/>
-    <numFmt formatCode="@" numFmtId="165"/>
   </numFmts>
   <fonts count="7">
     <font>
@@ -207,7 +200,7 @@
     <xf applyAlignment="false" applyBorder="false" applyFont="true" applyProtection="false" borderId="0" fillId="0" fontId="1" numFmtId="42"/>
     <xf applyAlignment="false" applyBorder="false" applyFont="true" applyProtection="false" borderId="0" fillId="0" fontId="1" numFmtId="9"/>
   </cellStyleXfs>
-  <cellXfs count="16">
+  <cellXfs count="15">
     <xf applyAlignment="false" applyBorder="false" applyFont="false" applyProtection="false" borderId="0" fillId="0" fontId="0" numFmtId="164" xfId="0"/>
     <xf applyAlignment="true" applyBorder="true" applyFont="true" applyProtection="false" borderId="1" fillId="2" fontId="4" numFmtId="164" xfId="0">
       <alignment horizontal="center" indent="0" shrinkToFit="false" textRotation="0" vertical="center" wrapText="false"/>
@@ -241,9 +234,6 @@
     </xf>
     <xf applyAlignment="true" applyBorder="false" applyFont="true" applyProtection="false" borderId="0" fillId="0" fontId="6" numFmtId="164" xfId="0">
       <alignment horizontal="left" indent="0" shrinkToFit="false" textRotation="0" vertical="top" wrapText="true"/>
-    </xf>
-    <xf applyAlignment="true" applyBorder="false" applyFont="true" applyProtection="false" borderId="0" fillId="0" fontId="6" numFmtId="165" xfId="0">
-      <alignment horizontal="right" indent="0" shrinkToFit="false" textRotation="0" vertical="top" wrapText="true"/>
     </xf>
     <xf applyAlignment="true" applyBorder="false" applyFont="true" applyProtection="false" borderId="0" fillId="0" fontId="6" numFmtId="164" xfId="0">
       <alignment horizontal="right" indent="0" shrinkToFit="false" textRotation="0" vertical="top" wrapText="false"/>
@@ -271,21 +261,19 @@
   <sheetPr filterMode="false">
     <pageSetUpPr fitToPage="false"/>
   </sheetPr>
-  <dimension ref="A1:H22"/>
+  <dimension ref="1:21"/>
   <sheetViews>
     <sheetView colorId="64" defaultGridColor="true" rightToLeft="false" showFormulas="false" showGridLines="true" showOutlineSymbols="true" showRowColHeaders="true" showZeros="true" tabSelected="true" topLeftCell="A1" view="normal" windowProtection="false" workbookViewId="0" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100">
       <selection activeCell="A1" activeCellId="0" pane="topLeft" sqref="A1"/>
     </sheetView>
   </sheetViews>
   <cols>
-    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="11.956862745098"/>
-    <col collapsed="false" hidden="false" max="2" min="2" style="0" width="40.2666666666667"/>
-    <col collapsed="false" hidden="false" max="3" min="3" style="0" width="11.8117647058824"/>
-    <col collapsed="false" hidden="false" max="5" min="4" style="0" width="40.2666666666667"/>
-    <col collapsed="false" hidden="false" max="6" min="6" style="0" width="11.956862745098"/>
-    <col collapsed="false" hidden="false" max="7" min="7" style="0" width="2.66666666666667"/>
-    <col collapsed="false" hidden="false" max="8" min="8" style="0" width="20.1960784313725"/>
-    <col collapsed="false" hidden="false" max="1025" min="9" style="0" width="11.8117647058824"/>
+    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="3.56470588235294"/>
+    <col collapsed="false" hidden="false" max="4" min="2" style="0" width="40.4627450980392"/>
+    <col collapsed="false" hidden="false" max="5" min="5" style="0" width="12.0196078431373"/>
+    <col collapsed="false" hidden="false" max="6" min="6" style="0" width="2.68627450980392"/>
+    <col collapsed="false" hidden="false" max="7" min="7" style="0" width="20.2941176470588"/>
+    <col collapsed="false" hidden="false" max="1025" min="8" style="0" width="11.8666666666667"/>
   </cols>
   <sheetData>
     <row collapsed="false" customFormat="true" customHeight="false" hidden="false" ht="14.95" outlineLevel="0" r="1" s="2">
@@ -298,19 +286,19 @@
       <c r="E1" s="1"/>
       <c r="F1" s="1"/>
       <c r="G1" s="1"/>
-      <c r="H1" s="1"/>
+      <c r="AMJ1" s="0"/>
     </row>
     <row collapsed="false" customFormat="true" customHeight="false" hidden="false" ht="14.95" outlineLevel="0" r="2" s="2">
       <c r="A2" s="3"/>
       <c r="B2" s="4"/>
-      <c r="C2" s="3"/>
+      <c r="C2" s="5"/>
       <c r="D2" s="5"/>
-      <c r="E2" s="5"/>
-      <c r="F2" s="6"/>
-      <c r="H2" s="7" t="n">
-        <f aca="false">SUM(H4:H22)</f>
-        <v>27.5</v>
-      </c>
+      <c r="E2" s="6"/>
+      <c r="G2" s="7" t="n">
+        <f aca="false">SUM(G4:G21)</f>
+        <v>26.5</v>
+      </c>
+      <c r="AMJ2" s="0"/>
     </row>
     <row collapsed="false" customFormat="true" customHeight="true" hidden="false" ht="38.9" outlineLevel="0" r="3" s="2">
       <c r="A3" s="1" t="s">
@@ -319,344 +307,325 @@
       <c r="B3" s="8" t="s">
         <v>2</v>
       </c>
-      <c r="C3" s="1" t="s">
+      <c r="C3" s="8" t="s">
         <v>3</v>
       </c>
       <c r="D3" s="8" t="s">
         <v>4</v>
       </c>
-      <c r="E3" s="8" t="s">
+      <c r="E3" s="1" t="s">
         <v>5</v>
       </c>
-      <c r="F3" s="1" t="s">
+      <c r="G3" s="8" t="s">
         <v>6</v>
       </c>
-      <c r="H3" s="8" t="s">
-        <v>7</v>
-      </c>
+      <c r="AMJ3" s="0"/>
     </row>
     <row collapsed="false" customFormat="true" customHeight="false" hidden="false" ht="14.15" outlineLevel="0" r="4" s="2">
       <c r="A4" s="9" t="n">
         <v>1</v>
       </c>
       <c r="B4" s="10" t="s">
-        <v>8</v>
-      </c>
-      <c r="C4" s="9"/>
+        <v>7</v>
+      </c>
+      <c r="C4" s="10"/>
       <c r="D4" s="10"/>
-      <c r="E4" s="10"/>
-      <c r="F4" s="9" t="n">
-        <v>1</v>
-      </c>
-      <c r="H4" s="7" t="n">
+      <c r="E4" s="9" t="n">
+        <v>1</v>
+      </c>
+      <c r="G4" s="7" t="n">
         <v>1.5</v>
       </c>
+      <c r="AMJ4" s="0"/>
     </row>
     <row collapsed="false" customFormat="true" customHeight="false" hidden="false" ht="14.15" outlineLevel="0" r="5" s="2">
       <c r="A5" s="9" t="n">
         <v>2</v>
       </c>
       <c r="B5" s="10" t="s">
-        <v>9</v>
-      </c>
-      <c r="C5" s="9"/>
+        <v>8</v>
+      </c>
+      <c r="C5" s="10"/>
       <c r="D5" s="10"/>
-      <c r="E5" s="10"/>
-      <c r="F5" s="9" t="n">
-        <v>1</v>
-      </c>
-      <c r="H5" s="7" t="n">
-        <v>1</v>
-      </c>
+      <c r="E5" s="9" t="n">
+        <v>1</v>
+      </c>
+      <c r="G5" s="7" t="n">
+        <v>1</v>
+      </c>
+      <c r="AMJ5" s="0"/>
     </row>
     <row collapsed="false" customFormat="true" customHeight="false" hidden="false" ht="26.65" outlineLevel="0" r="6" s="2">
       <c r="A6" s="9" t="n">
         <v>3</v>
       </c>
       <c r="B6" s="10" t="s">
-        <v>10</v>
-      </c>
-      <c r="C6" s="9"/>
+        <v>9</v>
+      </c>
+      <c r="C6" s="10"/>
       <c r="D6" s="10"/>
-      <c r="E6" s="10"/>
-      <c r="F6" s="9" t="n">
-        <v>1</v>
-      </c>
-      <c r="H6" s="7" t="n">
-        <v>1</v>
-      </c>
-    </row>
-    <row collapsed="false" customFormat="true" customHeight="false" hidden="false" ht="14.15" outlineLevel="0" r="7" s="14">
+      <c r="E6" s="9" t="n">
+        <v>1</v>
+      </c>
+      <c r="G6" s="7" t="n">
+        <v>1</v>
+      </c>
+      <c r="AMJ6" s="0"/>
+    </row>
+    <row collapsed="false" customFormat="true" customHeight="false" hidden="false" ht="14.15" outlineLevel="0" r="7" s="13">
       <c r="A7" s="9" t="n">
         <v>8</v>
       </c>
       <c r="B7" s="11" t="s">
-        <v>11</v>
-      </c>
-      <c r="C7" s="12"/>
+        <v>10</v>
+      </c>
+      <c r="C7" s="11"/>
       <c r="D7" s="11"/>
-      <c r="E7" s="11"/>
-      <c r="F7" s="13" t="n">
-        <v>1</v>
-      </c>
-      <c r="H7" s="13"/>
-    </row>
-    <row collapsed="false" customFormat="true" customHeight="false" hidden="false" ht="26.65" outlineLevel="0" r="8" s="14">
+      <c r="E7" s="12" t="n">
+        <v>1</v>
+      </c>
+      <c r="G7" s="12"/>
+      <c r="AMJ7" s="0"/>
+    </row>
+    <row collapsed="false" customFormat="true" customHeight="false" hidden="false" ht="26.65" outlineLevel="0" r="8" s="13">
       <c r="A8" s="9" t="n">
         <v>9</v>
       </c>
       <c r="B8" s="11" t="s">
-        <v>12</v>
-      </c>
-      <c r="C8" s="12"/>
+        <v>11</v>
+      </c>
+      <c r="C8" s="11"/>
       <c r="D8" s="11"/>
-      <c r="E8" s="11"/>
-      <c r="F8" s="13" t="n">
-        <v>1</v>
-      </c>
-      <c r="H8" s="13" t="n">
+      <c r="E8" s="12" t="n">
+        <v>1</v>
+      </c>
+      <c r="G8" s="12" t="n">
         <v>1.5</v>
       </c>
-    </row>
-    <row collapsed="false" customFormat="true" customHeight="false" hidden="false" ht="14.15" outlineLevel="0" r="9" s="14">
+      <c r="AMJ8" s="0"/>
+    </row>
+    <row collapsed="false" customFormat="true" customHeight="false" hidden="false" ht="14.15" outlineLevel="0" r="9" s="13">
       <c r="A9" s="9" t="n">
         <v>10</v>
       </c>
       <c r="B9" s="11" t="s">
-        <v>13</v>
-      </c>
-      <c r="C9" s="12"/>
+        <v>12</v>
+      </c>
+      <c r="C9" s="11"/>
       <c r="D9" s="11"/>
-      <c r="E9" s="11"/>
-      <c r="F9" s="13" t="n">
-        <v>1</v>
-      </c>
-      <c r="H9" s="13" t="n">
-        <v>2</v>
-      </c>
+      <c r="E9" s="12" t="n">
+        <v>1</v>
+      </c>
+      <c r="G9" s="12" t="n">
+        <v>2</v>
+      </c>
+      <c r="AMJ9" s="0"/>
     </row>
     <row collapsed="false" customFormat="true" customHeight="false" hidden="false" ht="14.15" outlineLevel="0" r="10" s="2">
       <c r="A10" s="9" t="n">
         <v>11</v>
       </c>
-      <c r="B10" s="15" t="s">
-        <v>14</v>
-      </c>
-      <c r="C10" s="7"/>
-      <c r="D10" s="15"/>
-      <c r="E10" s="15"/>
-      <c r="F10" s="7" t="n">
-        <v>2</v>
-      </c>
-      <c r="H10" s="7" t="n">
-        <v>3</v>
-      </c>
-    </row>
-    <row collapsed="false" customFormat="true" customHeight="false" hidden="false" ht="26.65" outlineLevel="0" r="11" s="14">
+      <c r="B10" s="14" t="s">
+        <v>13</v>
+      </c>
+      <c r="C10" s="14"/>
+      <c r="D10" s="14"/>
+      <c r="E10" s="7" t="n">
+        <v>2</v>
+      </c>
+      <c r="G10" s="7" t="n">
+        <v>3</v>
+      </c>
+      <c r="AMJ10" s="0"/>
+    </row>
+    <row collapsed="false" customFormat="true" customHeight="false" hidden="false" ht="26.65" outlineLevel="0" r="11" s="13">
       <c r="A11" s="9" t="n">
         <v>12</v>
       </c>
       <c r="B11" s="11" t="s">
-        <v>15</v>
-      </c>
-      <c r="C11" s="12"/>
+        <v>14</v>
+      </c>
+      <c r="C11" s="11"/>
       <c r="D11" s="11"/>
-      <c r="E11" s="11"/>
-      <c r="F11" s="13" t="n">
-        <v>2</v>
-      </c>
-      <c r="H11" s="13" t="n">
-        <v>2</v>
-      </c>
-    </row>
-    <row collapsed="false" customFormat="true" customHeight="false" hidden="false" ht="26.65" outlineLevel="0" r="12" s="14">
+      <c r="E11" s="12" t="n">
+        <v>2</v>
+      </c>
+      <c r="G11" s="12" t="n">
+        <v>2</v>
+      </c>
+      <c r="AMJ11" s="0"/>
+    </row>
+    <row collapsed="false" customFormat="true" customHeight="false" hidden="false" ht="26.65" outlineLevel="0" r="12" s="13">
       <c r="A12" s="9" t="n">
         <v>13</v>
       </c>
       <c r="B12" s="11" t="s">
-        <v>16</v>
-      </c>
-      <c r="C12" s="12"/>
+        <v>15</v>
+      </c>
+      <c r="C12" s="11"/>
       <c r="D12" s="11"/>
-      <c r="E12" s="11"/>
-      <c r="F12" s="13" t="n">
-        <v>2</v>
-      </c>
-      <c r="H12" s="13" t="n">
-        <v>1</v>
-      </c>
-    </row>
-    <row collapsed="false" customFormat="true" customHeight="false" hidden="false" ht="26.65" outlineLevel="0" r="13" s="14">
+      <c r="E12" s="12" t="n">
+        <v>2</v>
+      </c>
+      <c r="G12" s="12" t="n">
+        <v>1</v>
+      </c>
+      <c r="AMJ12" s="0"/>
+    </row>
+    <row collapsed="false" customFormat="true" customHeight="false" hidden="false" ht="26.65" outlineLevel="0" r="13" s="13">
       <c r="A13" s="9" t="n">
         <v>14</v>
       </c>
       <c r="B13" s="11" t="s">
-        <v>17</v>
-      </c>
-      <c r="C13" s="12"/>
+        <v>16</v>
+      </c>
+      <c r="C13" s="11"/>
       <c r="D13" s="11"/>
-      <c r="E13" s="11"/>
-      <c r="F13" s="13" t="n">
-        <v>2</v>
-      </c>
-      <c r="H13" s="13" t="n">
-        <v>2</v>
-      </c>
-    </row>
-    <row collapsed="false" customFormat="true" customHeight="false" hidden="false" ht="26.65" outlineLevel="0" r="14" s="14">
+      <c r="E13" s="12" t="n">
+        <v>2</v>
+      </c>
+      <c r="G13" s="12" t="n">
+        <v>2</v>
+      </c>
+      <c r="AMJ13" s="0"/>
+    </row>
+    <row collapsed="false" customFormat="true" customHeight="false" hidden="false" ht="26.65" outlineLevel="0" r="14" s="13">
       <c r="A14" s="9" t="n">
         <v>15</v>
       </c>
       <c r="B14" s="11" t="s">
-        <v>18</v>
-      </c>
-      <c r="C14" s="12"/>
+        <v>17</v>
+      </c>
+      <c r="C14" s="11"/>
       <c r="D14" s="11"/>
-      <c r="E14" s="11"/>
-      <c r="F14" s="13" t="n">
-        <v>2</v>
-      </c>
-      <c r="H14" s="13" t="n">
-        <v>2</v>
-      </c>
-    </row>
-    <row collapsed="false" customFormat="true" customHeight="false" hidden="false" ht="14.15" outlineLevel="0" r="15" s="14">
+      <c r="E14" s="12" t="n">
+        <v>2</v>
+      </c>
+      <c r="G14" s="12" t="n">
+        <v>2</v>
+      </c>
+      <c r="AMJ14" s="0"/>
+    </row>
+    <row collapsed="false" customFormat="true" customHeight="false" hidden="false" ht="14.15" outlineLevel="0" r="15" s="13">
       <c r="A15" s="9" t="n">
         <v>17</v>
       </c>
       <c r="B15" s="11" t="s">
-        <v>19</v>
-      </c>
-      <c r="C15" s="12"/>
+        <v>18</v>
+      </c>
+      <c r="C15" s="11"/>
       <c r="D15" s="11"/>
-      <c r="E15" s="11"/>
-      <c r="F15" s="13" t="n">
-        <v>3</v>
-      </c>
-      <c r="H15" s="13"/>
-    </row>
-    <row collapsed="false" customFormat="true" customHeight="false" hidden="false" ht="26.65" outlineLevel="0" r="16" s="14">
+      <c r="E15" s="12" t="n">
+        <v>3</v>
+      </c>
+      <c r="G15" s="12"/>
+      <c r="AMJ15" s="0"/>
+    </row>
+    <row collapsed="false" customFormat="true" customHeight="false" hidden="false" ht="26.65" outlineLevel="0" r="16" s="13">
       <c r="A16" s="9" t="n">
         <v>18</v>
       </c>
       <c r="B16" s="11" t="s">
-        <v>20</v>
-      </c>
-      <c r="C16" s="12"/>
+        <v>19</v>
+      </c>
+      <c r="C16" s="11"/>
       <c r="D16" s="11"/>
-      <c r="E16" s="11"/>
-      <c r="F16" s="13" t="n">
-        <v>3</v>
-      </c>
-      <c r="H16" s="13" t="n">
-        <v>2</v>
-      </c>
+      <c r="E16" s="12" t="n">
+        <v>3</v>
+      </c>
+      <c r="G16" s="12" t="n">
+        <v>2</v>
+      </c>
+      <c r="AMJ16" s="0"/>
     </row>
     <row collapsed="false" customFormat="true" customHeight="false" hidden="false" ht="26.65" outlineLevel="0" r="17" s="2">
       <c r="A17" s="9" t="n">
         <v>19</v>
       </c>
-      <c r="B17" s="15" t="s">
-        <v>21</v>
-      </c>
-      <c r="C17" s="7"/>
-      <c r="D17" s="15"/>
-      <c r="E17" s="15"/>
-      <c r="F17" s="7" t="n">
-        <v>3</v>
-      </c>
-      <c r="H17" s="7" t="n">
-        <v>2</v>
-      </c>
+      <c r="B17" s="14" t="s">
+        <v>20</v>
+      </c>
+      <c r="C17" s="14"/>
+      <c r="D17" s="14"/>
+      <c r="E17" s="7" t="n">
+        <v>3</v>
+      </c>
+      <c r="G17" s="7" t="n">
+        <v>2</v>
+      </c>
+      <c r="AMJ17" s="0"/>
     </row>
     <row collapsed="false" customFormat="true" customHeight="false" hidden="false" ht="14.15" outlineLevel="0" r="18" s="2">
       <c r="A18" s="9" t="n">
         <v>20</v>
       </c>
-      <c r="B18" s="15" t="s">
-        <v>22</v>
-      </c>
-      <c r="C18" s="7"/>
-      <c r="D18" s="15"/>
-      <c r="E18" s="15"/>
-      <c r="F18" s="7" t="n">
-        <v>3</v>
-      </c>
-      <c r="H18" s="7" t="n">
+      <c r="B18" s="14" t="s">
+        <v>21</v>
+      </c>
+      <c r="C18" s="14"/>
+      <c r="D18" s="14"/>
+      <c r="E18" s="7" t="n">
+        <v>3</v>
+      </c>
+      <c r="G18" s="7" t="n">
         <v>1.5</v>
       </c>
+      <c r="AMJ18" s="0"/>
     </row>
     <row collapsed="false" customFormat="true" customHeight="false" hidden="false" ht="26.65" outlineLevel="0" r="19" s="2">
       <c r="A19" s="9" t="n">
         <v>21</v>
       </c>
-      <c r="B19" s="15" t="s">
-        <v>23</v>
-      </c>
-      <c r="C19" s="7"/>
-      <c r="D19" s="15"/>
-      <c r="E19" s="15"/>
-      <c r="F19" s="7" t="n">
-        <v>3</v>
-      </c>
-      <c r="H19" s="7" t="n">
-        <v>1</v>
-      </c>
+      <c r="B19" s="14" t="s">
+        <v>22</v>
+      </c>
+      <c r="C19" s="14"/>
+      <c r="D19" s="14"/>
+      <c r="E19" s="7" t="n">
+        <v>3</v>
+      </c>
+      <c r="G19" s="7" t="n">
+        <v>1</v>
+      </c>
+      <c r="AMJ19" s="0"/>
     </row>
     <row collapsed="false" customFormat="true" customHeight="false" hidden="false" ht="26.65" outlineLevel="0" r="20" s="2">
       <c r="A20" s="9" t="n">
         <v>22</v>
       </c>
-      <c r="B20" s="15" t="s">
-        <v>24</v>
-      </c>
-      <c r="C20" s="7"/>
-      <c r="D20" s="15"/>
-      <c r="E20" s="15"/>
-      <c r="F20" s="7" t="n">
-        <v>3</v>
-      </c>
-      <c r="H20" s="7" t="n">
-        <v>2</v>
-      </c>
+      <c r="B20" s="14" t="s">
+        <v>23</v>
+      </c>
+      <c r="C20" s="14"/>
+      <c r="D20" s="14"/>
+      <c r="E20" s="7" t="n">
+        <v>3</v>
+      </c>
+      <c r="G20" s="7" t="n">
+        <v>2</v>
+      </c>
+      <c r="AMJ20" s="0"/>
     </row>
     <row collapsed="false" customFormat="true" customHeight="false" hidden="false" ht="14.15" outlineLevel="0" r="21" s="2">
       <c r="A21" s="9" t="n">
         <v>23</v>
       </c>
       <c r="B21" s="11" t="s">
-        <v>25</v>
-      </c>
-      <c r="C21" s="7"/>
-      <c r="D21" s="15"/>
-      <c r="E21" s="15"/>
-      <c r="F21" s="7" t="n">
-        <v>3</v>
-      </c>
-      <c r="H21" s="7" t="n">
-        <v>1</v>
-      </c>
-    </row>
-    <row collapsed="false" customFormat="true" customHeight="false" hidden="false" ht="14.15" outlineLevel="0" r="22" s="2">
-      <c r="A22" s="9" t="n">
         <v>24</v>
       </c>
-      <c r="B22" s="11" t="s">
-        <v>26</v>
-      </c>
-      <c r="C22" s="7"/>
-      <c r="D22" s="15"/>
-      <c r="E22" s="15"/>
-      <c r="F22" s="7" t="n">
-        <v>3</v>
-      </c>
-      <c r="H22" s="7" t="n">
-        <v>1</v>
-      </c>
+      <c r="C21" s="14"/>
+      <c r="D21" s="14"/>
+      <c r="E21" s="7" t="n">
+        <v>3</v>
+      </c>
+      <c r="G21" s="7" t="n">
+        <v>1</v>
+      </c>
+      <c r="AMJ21" s="0"/>
     </row>
   </sheetData>
   <mergeCells count="1">
-    <mergeCell ref="A1:H1"/>
+    <mergeCell ref="A1:G1"/>
   </mergeCells>
   <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>
   <pageMargins left="0.7875" right="0.7875" top="1.05277777777778" bottom="1.05277777777778" header="0.7875" footer="0.7875"/>

</xml_diff>